<commit_message>
Expand import validation in MCC
</commit_message>
<xml_diff>
--- a/mcc/resources/web/mcc/exampleData/MCC_Data_Template.xlsx
+++ b/mcc/resources/web/mcc/exampleData/MCC_Data_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20388"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bimber\Desktop\MCC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\discvr-lk\server\modules\BimberLabKeyModules\mcc\resources\web\mcc\exampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90528A6E-65BE-4318-9E06-74ECF625CDDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AAB6AF-94AB-4CC1-BD4A-FFD65A843462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>sex</t>
   </si>
@@ -152,6 +152,30 @@
   </si>
   <si>
     <t>In order to have a robust database of marmosets, the MCC requires a set of minimal data to enroll an animal. Please fill out the "animal data" worksheet, listing each animal in a new row.</t>
+  </si>
+  <si>
+    <t>1 - female</t>
+  </si>
+  <si>
+    <t>1 - assigned to U24 breeding colong</t>
+  </si>
+  <si>
+    <t>1 - available for transfer</t>
+  </si>
+  <si>
+    <t>1 - natal family group</t>
+  </si>
+  <si>
+    <t>1 - sibling experience only</t>
+  </si>
+  <si>
+    <t>1 - mated no offspring produced</t>
+  </si>
+  <si>
+    <t>1 - animal assigned to invasive study</t>
+  </si>
+  <si>
+    <t>available to transfer</t>
   </si>
 </sst>
 </file>
@@ -202,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -236,7 +260,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -620,11 +643,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="12" t="s">
@@ -740,7 +763,7 @@
       <c r="A17" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17" t="s">
@@ -751,7 +774,7 @@
       <c r="A18" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
       <c r="C18" t="s">
@@ -829,7 +852,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
@@ -880,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>3</v>
@@ -896,50 +919,95 @@
       </c>
       <c r="P1" s="11"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" ht="45">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16">
       <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
       <c r="P5" s="3"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
       <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
       <c r="P7" s="3"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
       <c r="P8" s="3"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16">
@@ -949,7 +1017,7 @@
       <c r="P13" s="3"/>
     </row>
     <row r="18" spans="4:17">
-      <c r="D18" s="14"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="21" spans="4:17">
       <c r="Q21" s="3"/>
@@ -959,28 +1027,29 @@
     </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"0 - male, 1 - female"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"0 - not assigned to U24 breeding colony, 1 - assigned to U24 breeding colong"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"0 - not available for transfer, 1 - available for transfer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"0 - singly housed, 1 - natal family group, 2 - active breeding, 3 - social non breeding"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{00000000-0002-0000-0100-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"0 - no experience, 1 - sibling experience only, 2 - non successful offspring, 3 - successful rearing of offspring"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576" xr:uid="{00000000-0002-0000-0100-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>"0 - no mating opportunity, 1 - mated no offspring produced, 2 - successful offspring produced, 3 - hormonal birth control, 4 - sterilized"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1:O1048576" xr:uid="{00000000-0002-0000-0100-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{00000000-0002-0000-0100-000006000000}">
       <formula1>"0 - naive animal, 1 - animal assigned to invasive study"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Expand import validation in MCC (#157)
* Expand import validation in MCC
</commit_message>
<xml_diff>
--- a/mcc/resources/web/mcc/exampleData/MCC_Data_Template.xlsx
+++ b/mcc/resources/web/mcc/exampleData/MCC_Data_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20388"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bimber\Desktop\MCC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\discvr-lk\server\modules\BimberLabKeyModules\mcc\resources\web\mcc\exampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90528A6E-65BE-4318-9E06-74ECF625CDDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AAB6AF-94AB-4CC1-BD4A-FFD65A843462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>sex</t>
   </si>
@@ -152,6 +152,30 @@
   </si>
   <si>
     <t>In order to have a robust database of marmosets, the MCC requires a set of minimal data to enroll an animal. Please fill out the "animal data" worksheet, listing each animal in a new row.</t>
+  </si>
+  <si>
+    <t>1 - female</t>
+  </si>
+  <si>
+    <t>1 - assigned to U24 breeding colong</t>
+  </si>
+  <si>
+    <t>1 - available for transfer</t>
+  </si>
+  <si>
+    <t>1 - natal family group</t>
+  </si>
+  <si>
+    <t>1 - sibling experience only</t>
+  </si>
+  <si>
+    <t>1 - mated no offspring produced</t>
+  </si>
+  <si>
+    <t>1 - animal assigned to invasive study</t>
+  </si>
+  <si>
+    <t>available to transfer</t>
   </si>
 </sst>
 </file>
@@ -202,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -236,7 +260,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -620,11 +643,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="12" t="s">
@@ -740,7 +763,7 @@
       <c r="A17" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17" t="s">
@@ -751,7 +774,7 @@
       <c r="A18" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
       <c r="C18" t="s">
@@ -829,7 +852,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
@@ -880,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>3</v>
@@ -896,50 +919,95 @@
       </c>
       <c r="P1" s="11"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" ht="45">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16">
       <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
       <c r="P5" s="3"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
       <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
       <c r="P7" s="3"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
       <c r="P8" s="3"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16">
@@ -949,7 +1017,7 @@
       <c r="P13" s="3"/>
     </row>
     <row r="18" spans="4:17">
-      <c r="D18" s="14"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="21" spans="4:17">
       <c r="Q21" s="3"/>
@@ -959,28 +1027,29 @@
     </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"0 - male, 1 - female"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"0 - not assigned to U24 breeding colony, 1 - assigned to U24 breeding colong"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"0 - not available for transfer, 1 - available for transfer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"0 - singly housed, 1 - natal family group, 2 - active breeding, 3 - social non breeding"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{00000000-0002-0000-0100-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"0 - no experience, 1 - sibling experience only, 2 - non successful offspring, 3 - successful rearing of offspring"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576" xr:uid="{00000000-0002-0000-0100-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>"0 - no mating opportunity, 1 - mated no offspring produced, 2 - successful offspring produced, 3 - hormonal birth control, 4 - sterilized"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1:O1048576" xr:uid="{00000000-0002-0000-0100-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{00000000-0002-0000-0100-000006000000}">
       <formula1>"0 - naive animal, 1 - animal assigned to invasive study"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>